<commit_message>
da xong check out va sua create o 2 ben, da co luu history bang BE, tiêp tuc dang chen history cho cac thay doi>
</commit_message>
<xml_diff>
--- a/backend/exports/Báo-cáo-doanh-thu-Tháng-11-2024.xlsx
+++ b/backend/exports/Báo-cáo-doanh-thu-Tháng-11-2024.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="68">
   <si>
     <t>BẢNG KÊ DOANH THU</t>
   </si>
@@ -76,31 +76,16 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>Phòng Đơn</t>
-  </si>
-  <si>
-    <t>500,000</t>
+    <t>Tổng:</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Phòng Đôi</t>
-  </si>
-  <si>
-    <t>800,000</t>
-  </si>
-  <si>
-    <t>Tổng:</t>
-  </si>
-  <si>
-    <t>1,300,000</t>
-  </si>
-  <si>
-    <t>Tổng doanh thu: 1,300,000</t>
+    <t>Tổng doanh thu: 0</t>
   </si>
   <si>
     <t>Số phòng:</t>
@@ -112,24 +97,9 @@
     <t>NGÀY 2/11/2024</t>
   </si>
   <si>
-    <t>Phòng Gia Đình</t>
-  </si>
-  <si>
-    <t>1,200,000</t>
-  </si>
-  <si>
-    <t>2,000,000</t>
-  </si>
-  <si>
-    <t>Tổng doanh thu: 2,000,000</t>
-  </si>
-  <si>
     <t>NGÀY 3/11/2024</t>
   </si>
   <si>
-    <t>Tổng doanh thu: 0</t>
-  </si>
-  <si>
     <t>NGÀY 4/11/2024</t>
   </si>
   <si>
@@ -157,33 +127,15 @@
     <t>NGÀY 12/11/2024</t>
   </si>
   <si>
-    <t>Standard Room</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>Tổng doanh thu: 80</t>
-  </si>
-  <si>
     <t>NGÀY 13/11/2024</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>NGÀY 14/11/2024</t>
   </si>
   <si>
     <t>NGÀY 15/11/2024</t>
   </si>
   <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>Tổng doanh thu: 85</t>
-  </si>
-  <si>
     <t>NGÀY 16/11/2024</t>
   </si>
   <si>
@@ -202,18 +154,54 @@
     <t>NGÀY 21/11/2024</t>
   </si>
   <si>
+    <t>phòng đôi</t>
+  </si>
+  <si>
+    <t>400,000</t>
+  </si>
+  <si>
+    <t>phòng VIP</t>
+  </si>
+  <si>
+    <t>450,000</t>
+  </si>
+  <si>
+    <t>8,650,000</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu: 8,650,000</t>
+  </si>
+  <si>
     <t>NGÀY 22/11/2024</t>
   </si>
   <si>
     <t>NGÀY 23/11/2024</t>
   </si>
   <si>
+    <t>850,000</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu: 850,000</t>
+  </si>
+  <si>
     <t>NGÀY 24/11/2024</t>
   </si>
   <si>
+    <t>4,650,000</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu: 4,650,000</t>
+  </si>
+  <si>
     <t>NGÀY 25/11/2024</t>
   </si>
   <si>
+    <t>1,250,000</t>
+  </si>
+  <si>
+    <t>Tổng doanh thu: 1,250,000</t>
+  </si>
+  <si>
     <t>NGÀY 26/11/2024</t>
   </si>
   <si>
@@ -247,22 +235,16 @@
     <t>Tổng doanh thu</t>
   </si>
   <si>
-    <t>1/11/2024</t>
-  </si>
-  <si>
-    <t>2/11/2024</t>
-  </si>
-  <si>
-    <t>12/11/2024</t>
-  </si>
-  <si>
-    <t>13/11/2024</t>
-  </si>
-  <si>
-    <t>14/11/2024</t>
-  </si>
-  <si>
-    <t>15/11/2024</t>
+    <t>21/11/2024</t>
+  </si>
+  <si>
+    <t>23/11/2024</t>
+  </si>
+  <si>
+    <t>24/11/2024</t>
+  </si>
+  <si>
+    <t>25/11/2024</t>
   </si>
 </sst>
 </file>
@@ -324,9 +306,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -727,111 +709,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -868,7 +792,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -910,51 +834,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -991,7 +915,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1033,51 +957,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1093,7 +1017,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -1114,7 +1038,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1154,82 +1078,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1245,7 +1140,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -1266,7 +1161,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1306,82 +1201,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1397,7 +1263,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -1418,7 +1284,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1458,82 +1324,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1549,7 +1386,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -1570,7 +1407,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1610,82 +1447,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1722,7 +1530,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1764,51 +1572,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1845,7 +1653,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1887,51 +1695,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1968,7 +1776,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2010,51 +1818,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2091,7 +1899,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2133,51 +1941,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2193,7 +2001,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -2214,7 +2022,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2254,111 +2062,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2395,7 +2145,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2437,51 +2187,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2497,7 +2247,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I28"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -2518,7 +2268,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2558,53 +2308,662 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>20</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>21</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2641,7 +3000,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2683,51 +3042,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2743,7 +3102,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -2764,7 +3123,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2804,53 +3163,111 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2866,7 +3283,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -2887,7 +3304,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2927,53 +3344,372 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2989,7 +3725,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="20" customWidth="1"/>
@@ -3010,7 +3746,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3050,53 +3786,140 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="4" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3133,7 +3956,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3175,51 +3998,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3256,7 +4079,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3298,51 +4121,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3379,7 +4202,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3421,51 +4244,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3502,7 +4325,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3544,51 +4367,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3625,7 +4448,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3667,51 +4490,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3748,7 +4571,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3790,51 +4613,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3850,7 +4673,7 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
@@ -3868,7 +4691,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3876,144 +4699,104 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" ht="25" customHeight="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" ht="25" customHeight="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="4" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C4" s="6">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>10250000</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="C6" s="6">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>9050000</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>4400000</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>85</v>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1250000</v>
       </c>
     </row>
   </sheetData>
@@ -4049,7 +4832,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4091,51 +4874,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4172,7 +4955,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4214,51 +4997,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4295,7 +5078,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4337,51 +5120,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4418,7 +5201,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4460,51 +5243,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4541,7 +5324,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4583,51 +5366,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4664,7 +5447,7 @@
     </row>
     <row r="2" ht="25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4706,51 +5489,51 @@
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" ht="25" customHeight="1" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6">
+    </row>
+    <row r="6" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>